<commit_message>
Add KPS and EQ5D
</commit_message>
<xml_diff>
--- a/curation/draft/package12/R12_BC_SDTM_QRS_ATLAS.xlsx
+++ b/curation/draft/package12/R12_BC_SDTM_QRS_ATLAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\package12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED737DA-4E55-4FF3-8E3F-D9A1454AC985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EBB7BC-2788-4668-BC6D-5789DAD9A002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1000,7 +1000,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,29 +1085,31 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="9"/>
+        <v>98</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
@@ -1120,31 +1122,29 @@
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
     </row>
-    <row r="3" spans="1:19" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>103</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>

</xml_diff>